<commit_message>
Koodien suunnittelutiedosto ja tyoajanseuranta
</commit_message>
<xml_diff>
--- a/Dokumentit/Projektin luokkien ja koodien suunnittelu.xlsx
+++ b/Dokumentit/Projektin luokkien ja koodien suunnittelu.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaana\source\repos\Ohjelmistokehitysprojekti\Dokumentit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1C88D8-B16B-4048-90A1-2D48CF14D0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24B0ADE-1F55-4811-8273-C69E1214006E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF39234B-C75A-4338-A701-D26E791B20F8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{BF39234B-C75A-4338-A701-D26E791B20F8}"/>
   </bookViews>
   <sheets>
     <sheet name="MainWindow.xaml.cs" sheetId="3" r:id="rId1"/>
-    <sheet name="Customer-luokka" sheetId="1" r:id="rId2"/>
-    <sheet name="ServiceLevel-luokka" sheetId="2" r:id="rId3"/>
-    <sheet name="ServiceLevelWindow.xaml.cs" sheetId="6" r:id="rId4"/>
-    <sheet name="CustomerWindow.xaml.cs" sheetId="7" r:id="rId5"/>
+    <sheet name="CustomerWindow.xaml.cs" sheetId="7" r:id="rId2"/>
+    <sheet name="ServiceLevelWindow.xaml.cs" sheetId="6" r:id="rId3"/>
+    <sheet name="Customer-luokka" sheetId="1" r:id="rId4"/>
+    <sheet name="Invoice-luokka" sheetId="8" r:id="rId5"/>
+    <sheet name="ServiceLevel-luokka" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="85">
   <si>
     <t>class Asiakas:</t>
   </si>
@@ -87,24 +88,15 @@
     <t>double</t>
   </si>
   <si>
-    <t>Uusi Palvelutaso -nappi</t>
-  </si>
-  <si>
     <t>property BillingDate</t>
   </si>
   <si>
     <t>Sulkee ikkunan</t>
   </si>
   <si>
-    <t>Lisää Asiakas -nappi</t>
-  </si>
-  <si>
     <t>luodaan uusi (Asiakkaan lisäys) Window -objekti</t>
   </si>
   <si>
-    <t>avataan uusi (Palvelutason lisäys) Window -objekti</t>
-  </si>
-  <si>
     <t>Luodaan uusi ServiceLevel-objekti</t>
   </si>
   <si>
@@ -168,24 +160,6 @@
     <t>Sulje -nappi</t>
   </si>
   <si>
-    <t>Muut valinnat:</t>
-  </si>
-  <si>
-    <t>Alennukset:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 kk: </t>
-  </si>
-  <si>
-    <t>12 kk:</t>
-  </si>
-  <si>
-    <t>kutsuu Discount6() -metodia</t>
-  </si>
-  <si>
-    <t>kutsuu Discount12() -metodia</t>
-  </si>
-  <si>
     <t>public void Discount6()</t>
   </si>
   <si>
@@ -195,24 +169,156 @@
     <t>public void TrialPeriod()</t>
   </si>
   <si>
-    <t>30 pv kokeilujakso:</t>
-  </si>
-  <si>
-    <t>kutsuu TrialPeriod() -metodia</t>
-  </si>
-  <si>
-    <t>Haetaan tiedot asiakkaiden tulevista maksuista customers.json-tiedostosta ja näytetään tulevat maksut MainWindowssa listaelementissä</t>
-  </si>
-  <si>
     <t>Tulostetaan maksujen tiedot tiedostoon billingdate.text</t>
+  </si>
+  <si>
+    <t>public class Invoice</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>public DateTime Invoicedate { get; set;}</t>
+  </si>
+  <si>
+    <t>public double InvoiceSum { get; set;)</t>
+  </si>
+  <si>
+    <t>public Customer CustomerName { get; set; }</t>
+  </si>
+  <si>
+    <t>InvoiceSum = sum;</t>
+  </si>
+  <si>
+    <t>CustomerName = name;</t>
+  </si>
+  <si>
+    <t>InvoiceDate = invoicedate;</t>
+  </si>
+  <si>
+    <t>public Invoice (DateTime invoicedate, int dateamount, double sum, Customer name)</t>
+  </si>
+  <si>
+    <t>InvoiceDate = invoicedate.AddDays(dateamount);</t>
+  </si>
+  <si>
+    <t>Lisää asiakas-nappula</t>
+  </si>
+  <si>
+    <t>Lisää palvelutaso -nappula</t>
+  </si>
+  <si>
+    <t>Laskut -nappula</t>
+  </si>
+  <si>
+    <t>Tulosta tiedostoon -nappula</t>
+  </si>
+  <si>
+    <t>MainWindow() -metodi</t>
+  </si>
+  <si>
+    <t>InitializeComponent()</t>
+  </si>
+  <si>
+    <t>luetaan invoices -JSON-tiedosto sisään ja deserialisoidaan lista-tyyppiseksi.</t>
+  </si>
+  <si>
+    <t>foreach-silmukalla lisätään jokainen listan itemeista listViewiin</t>
+  </si>
+  <si>
+    <t>näytetään asiakkaan lisäys-ikkuna</t>
+  </si>
+  <si>
+    <t>Lisää Asiakas -napin metodi</t>
+  </si>
+  <si>
+    <t>Uusi Palvelutaso -napin metodi</t>
+  </si>
+  <si>
+    <t>luodaan uusi (Palvelutason lisäys) Window -objekti</t>
+  </si>
+  <si>
+    <t>näytetään palvelutason lisäys -ikkuna</t>
+  </si>
+  <si>
+    <t>jossa näytetään maksupäivä, summa ja asiakkaan nimi</t>
+  </si>
+  <si>
+    <t>Tarkistetaan projektin edetessä tämän tarpeellisuus!</t>
+  </si>
+  <si>
+    <t>listView, johon tulee näkyviin maksupäivät, laskut ja asiakkaan nimi</t>
+  </si>
+  <si>
+    <t>MainWindown elementit</t>
+  </si>
+  <si>
+    <t>CustomerWindown elementit:</t>
+  </si>
+  <si>
+    <t>textboxit 5 kpl asiakkaan nimi, osoite, postinumero, kaupunki, sähköposti</t>
+  </si>
+  <si>
+    <t>datepicker laskutuspäivän valintaan</t>
+  </si>
+  <si>
+    <t>combobox palvelutason valintaan</t>
+  </si>
+  <si>
+    <t>combobox kausioston tai ilmaisen kokeilujakson valintaan</t>
+  </si>
+  <si>
+    <t>Tallenna ja Poistu -napit</t>
+  </si>
+  <si>
+    <t>listView jossa lista asiakkaista (nimi, osoite, kaupunki)</t>
+  </si>
+  <si>
+    <t>Poista ja Muokkaa -napit</t>
+  </si>
+  <si>
+    <t>textboxien GotFocus -metodit</t>
+  </si>
+  <si>
+    <t>Valitaan textboxin ohjeteksti sinne tab-painikkeella siirryttäessä</t>
+  </si>
+  <si>
+    <t>CustomerWindow() -metodi</t>
+  </si>
+  <si>
+    <t>Luetaan sisään servicelevels -json tiedosto ja deserialisoidaan se listaksi</t>
+  </si>
+  <si>
+    <t>foreach-silmukalla asetetaan jokainen listan objekti (Text-muuttuja) palvelutason comboboxin itemiksi</t>
+  </si>
+  <si>
+    <t>if (dateamount != 0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -240,8 +346,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -257,6 +366,153 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>20354</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>92647</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>135940</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Kuva 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D5C8579-19B5-E934-FD5B-B4222E2C6175}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6725954" y="125730"/>
+          <a:ext cx="7391303" cy="4168825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>174122</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>384082</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>172111</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Kuva 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C16D484-A36D-F351-B232-2F5E31658C11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7677149" y="174122"/>
+          <a:ext cx="6737258" cy="3794654"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>298303</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>116834</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Kuva 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E21E0995-BDB3-7FA4-9C46-04388D3D665A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7486650" y="314325"/>
+          <a:ext cx="8051653" cy="4507859"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -556,100 +812,342 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D93F0A-1BDF-4CF3-8C90-6D7803FB8C3F}">
-  <dimension ref="B1:C19"/>
+  <dimension ref="B1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35:O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>25</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>15</v>
+      <c r="C8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>30</v>
+      <c r="B11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L26" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L28" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429D0F54-E52D-45ED-BE09-7C2B5A8133C5}">
+  <dimension ref="B2:M31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M24" sqref="M24:M31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FF0A42-4DC3-49B8-BA24-EAEA2D2F54AA}">
+  <dimension ref="B1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94713E4B-84D9-4487-9649-265E4ED20987}">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -717,25 +1215,25 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -745,17 +1243,17 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
@@ -765,22 +1263,22 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -788,7 +1286,122 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4833F399-FC1A-4186-9C5E-5A1B012D833F}">
+  <dimension ref="A1:O19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9:O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="15" max="15" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="N9" s="3">
+        <v>44989</v>
+      </c>
+      <c r="O9" s="3">
+        <f>N9+180</f>
+        <v>45169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50138403-55CE-417B-83A2-7668390F721D}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -825,134 +1438,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FF0A42-4DC3-49B8-BA24-EAEA2D2F54AA}">
-  <dimension ref="B1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429D0F54-E52D-45ED-BE09-7C2B5A8133C5}">
-  <dimension ref="B1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>